<commit_message>
test: add new datatypes to example excel class
</commit_message>
<xml_diff>
--- a/src/test/resources/Fake_Employee_Data_Error.xlsx
+++ b/src/test/resources/Fake_Employee_Data_Error.xlsx
@@ -372,7 +372,7 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G17" activeCellId="0" sqref="G17"/>
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -407,7 +407,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
-        <v>1060</v>
+        <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>6</v>
@@ -481,7 +481,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
-        <v>4029</v>
+        <v>0</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>14</v>
@@ -499,7 +499,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
-        <v>6585</v>
+        <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>16</v>
@@ -537,7 +537,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
-        <v>5742</v>
+        <v>1</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>20</v>

</xml_diff>